<commit_message>
created Wonder-Config files for HUFO and 325
</commit_message>
<xml_diff>
--- a/speakerpositions/EN325-WFS/EN325_WFS_Panels.xlsx
+++ b/speakerpositions/EN325-WFS/EN325_WFS_Panels.xlsx
@@ -5,16 +5,17 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/psch/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/psch/Documents/GitHub/hufo_system/speakerpositions/EN325-WFS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{923CA7D9-665B-2540-8FF5-78303AB8A560}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{23706871-613C-CB42-BE1A-1675E6F18A14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{C770B271-DD15-0447-B9BA-73B85979A476}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{C770B271-DD15-0447-B9BA-73B85979A476}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="exportPanels" sheetId="2" r:id="rId2"/>
+    <sheet name="exportPolygon" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>Panel ID</t>
   </si>
@@ -123,13 +124,28 @@
   <si>
     <t>end Y</t>
   </si>
+  <si>
+    <t>Point</t>
+  </si>
+  <si>
+    <t>x1</t>
+  </si>
+  <si>
+    <t>y1</t>
+  </si>
+  <si>
+    <t>Polygon</t>
+  </si>
+  <si>
+    <t>wOffset</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -298,7 +314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -307,10 +323,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -318,6 +331,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -633,10 +652,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18754C6F-9105-7F4B-B6EF-4A5F1225395A}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:V32"/>
+  <dimension ref="A1:V44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="144" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:M26"/>
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -647,27 +666,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="G1" s="9" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="G1" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="O1" s="9" t="s">
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="O1" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
       <c r="T1" t="s">
         <v>24</v>
       </c>
@@ -779,25 +798,25 @@
       </c>
       <c r="O3" s="8">
         <f>J3 - ((G3/$I3) * ($G$31 / 2)) + $J$31</f>
-        <v>0.45500000000000007</v>
+        <v>5.5000000000000049E-2</v>
       </c>
       <c r="P3" s="8">
         <f>K3 - ((H3/$I3) * ($G$31 / 2)) + $J$31</f>
-        <v>3.423</v>
+        <v>3.0230000000000001</v>
       </c>
       <c r="Q3" s="8">
         <f>J3 + ((G3/$I3) * ($G$31 / 2)) + $J$31</f>
-        <v>1.155</v>
+        <v>0.755</v>
       </c>
       <c r="R3" s="8">
         <f>K3 + ((H3/$I3) * ($G$31 / 2)) + $J$31</f>
-        <v>3.423</v>
+        <v>3.0230000000000001</v>
       </c>
       <c r="T3">
         <v>1.4</v>
       </c>
       <c r="V3" s="8">
-        <f>(SQRT(POWER(Q3-O3,2)+POWER(R3-P3,2)))</f>
+        <f t="shared" ref="V3:V26" si="0">(SQRT(POWER(Q3-O3,2)+POWER(R3-P3,2)))</f>
         <v>0.7</v>
       </c>
     </row>
@@ -810,68 +829,68 @@
         <v>0.81</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C8" si="0">C27</f>
+        <f t="shared" ref="C4:C8" si="1">C27</f>
         <v>3.0230000000000001</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D25" si="1">B5</f>
+        <f t="shared" ref="D4:D25" si="2">B5</f>
         <v>1.62</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E25" si="2">C5</f>
+        <f t="shared" ref="E4:E25" si="3">C5</f>
         <v>3.0230000000000001</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="8">
-        <f t="shared" ref="G4:G26" si="3">D4 - B4</f>
+        <f t="shared" ref="G4:G26" si="4">D4 - B4</f>
         <v>0.81</v>
       </c>
       <c r="H4" s="8">
-        <f t="shared" ref="H4:H26" si="4" xml:space="preserve"> E4 - C4</f>
+        <f t="shared" ref="H4:H26" si="5" xml:space="preserve"> E4 - C4</f>
         <v>0</v>
       </c>
       <c r="I4" s="8">
-        <f t="shared" ref="I4:I26" si="5" xml:space="preserve"> SQRT(POWER(G4,2) + POWER(H4,2))</f>
+        <f t="shared" ref="I4:I26" si="6" xml:space="preserve"> SQRT(POWER(G4,2) + POWER(H4,2))</f>
         <v>0.81</v>
       </c>
       <c r="J4" s="8">
-        <f t="shared" ref="J4:J26" si="6" xml:space="preserve"> B4 + (G4 / 2)</f>
+        <f t="shared" ref="J4:J26" si="7" xml:space="preserve"> B4 + (G4 / 2)</f>
         <v>1.2150000000000001</v>
       </c>
       <c r="K4" s="8">
-        <f t="shared" ref="K4:K26" si="7" xml:space="preserve"> C4 + (H4 / 2)</f>
+        <f t="shared" ref="K4:K26" si="8" xml:space="preserve"> C4 + (H4 / 2)</f>
         <v>3.0230000000000001</v>
       </c>
       <c r="L4" s="8">
-        <f t="shared" ref="L4:L26" si="8">H4 / I4</f>
+        <f t="shared" ref="L4:L26" si="9">H4 / I4</f>
         <v>0</v>
       </c>
       <c r="M4" s="8">
-        <f t="shared" ref="M4:M26" si="9" xml:space="preserve"> -G4 / I4</f>
+        <f t="shared" ref="M4:M26" si="10" xml:space="preserve"> -G4 / I4</f>
         <v>-1</v>
       </c>
       <c r="O4" s="8">
-        <f t="shared" ref="O4:O26" si="10">J4 - ((G4/$I4) * ($G$31 / 2)) + $J$31</f>
-        <v>1.2650000000000001</v>
+        <f t="shared" ref="O4:O26" si="11">J4 - ((G4/$I4) * ($G$31 / 2)) + $J$31</f>
+        <v>0.8650000000000001</v>
       </c>
       <c r="P4" s="8">
-        <f t="shared" ref="P4:P26" si="11">K4 - ((H4/$I4) * ($G$31 / 2)) + $J$31</f>
-        <v>3.423</v>
+        <f t="shared" ref="P4:P26" si="12">K4 - ((H4/$I4) * ($G$31 / 2)) + $J$31</f>
+        <v>3.0230000000000001</v>
       </c>
       <c r="Q4" s="8">
-        <f t="shared" ref="Q4:Q26" si="12">J4 + ((G4/$I4) * ($G$31 / 2)) + $J$31</f>
-        <v>1.9649999999999999</v>
+        <f t="shared" ref="Q4:Q26" si="13">J4 + ((G4/$I4) * ($G$31 / 2)) + $J$31</f>
+        <v>1.5649999999999999</v>
       </c>
       <c r="R4" s="8">
-        <f t="shared" ref="R4:R26" si="13">K4 + ((H4/$I4) * ($G$31 / 2)) + $J$31</f>
-        <v>3.423</v>
+        <f t="shared" ref="R4:R26" si="14">K4 + ((H4/$I4) * ($G$31 / 2)) + $J$31</f>
+        <v>3.0230000000000001</v>
       </c>
       <c r="T4">
         <v>1.4</v>
       </c>
       <c r="V4" s="8">
-        <f>(SQRT(POWER(Q4-O4,2)+POWER(R4-P4,2)))</f>
-        <v>0.69999999999999973</v>
+        <f t="shared" si="0"/>
+        <v>0.69999999999999984</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
@@ -883,67 +902,67 @@
         <v>1.62</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.0230000000000001</v>
       </c>
       <c r="D5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.0249999999999999</v>
       </c>
       <c r="E5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.3214999999999999</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.4049999999999998</v>
       </c>
       <c r="H5" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-0.70150000000000023</v>
       </c>
       <c r="I5" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.8100168208130003</v>
       </c>
       <c r="J5" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.8225</v>
       </c>
       <c r="K5" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.67225</v>
       </c>
       <c r="L5" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.86603139833061304</v>
       </c>
       <c r="M5" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-0.49998961699771627</v>
       </c>
       <c r="O5" s="8">
-        <f t="shared" si="10"/>
-        <v>2.0475036340507993</v>
+        <f t="shared" si="11"/>
+        <v>1.6475036340507994</v>
       </c>
       <c r="P5" s="8">
-        <f t="shared" si="11"/>
-        <v>3.3753609894157144</v>
+        <f t="shared" si="12"/>
+        <v>2.9753609894157145</v>
       </c>
       <c r="Q5" s="8">
-        <f t="shared" si="12"/>
-        <v>2.3974963659492006</v>
+        <f t="shared" si="13"/>
+        <v>1.9974963659492007</v>
       </c>
       <c r="R5" s="8">
-        <f t="shared" si="13"/>
-        <v>2.7691390105842855</v>
+        <f t="shared" si="14"/>
+        <v>2.3691390105842856</v>
       </c>
       <c r="T5">
         <v>1.4</v>
       </c>
       <c r="V5" s="8">
-        <f>(SQRT(POWER(Q5-O5,2)+POWER(R5-P5,2)))</f>
+        <f t="shared" si="0"/>
         <v>0.69999999999999973</v>
       </c>
     </row>
@@ -956,68 +975,68 @@
         <v>2.0249999999999999</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.3214999999999999</v>
       </c>
       <c r="D6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.4300000000000002</v>
       </c>
       <c r="E6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.62</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.40500000000000025</v>
       </c>
       <c r="H6" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-0.70149999999999979</v>
       </c>
       <c r="I6" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.81001682081300008</v>
       </c>
       <c r="J6" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.2275</v>
       </c>
       <c r="K6" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.97075</v>
       </c>
       <c r="L6" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.86603139833061271</v>
       </c>
       <c r="M6" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-0.49998961699771699</v>
       </c>
       <c r="O6" s="8">
-        <f t="shared" si="10"/>
-        <v>2.4525036340507991</v>
+        <f t="shared" si="11"/>
+        <v>2.0525036340507992</v>
       </c>
       <c r="P6" s="8">
-        <f t="shared" si="11"/>
-        <v>2.6738609894157142</v>
+        <f t="shared" si="12"/>
+        <v>2.2738609894157142</v>
       </c>
       <c r="Q6" s="8">
-        <f t="shared" si="12"/>
-        <v>2.8024963659492008</v>
+        <f t="shared" si="13"/>
+        <v>2.4024963659492009</v>
       </c>
       <c r="R6" s="8">
-        <f t="shared" si="13"/>
-        <v>2.0676390105842857</v>
+        <f t="shared" si="14"/>
+        <v>1.6676390105842855</v>
       </c>
       <c r="T6">
         <v>1.4</v>
       </c>
       <c r="V6" s="8">
-        <f>(SQRT(POWER(Q6-O6,2)+POWER(R6-P6,2)))</f>
-        <v>0.69999999999999962</v>
+        <f t="shared" si="0"/>
+        <v>0.69999999999999984</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
@@ -1025,72 +1044,72 @@
         <v>105</v>
       </c>
       <c r="B7">
-        <f t="shared" ref="B5:B8" si="14">B30*-1</f>
+        <f t="shared" ref="B7:B8" si="15">B30*-1</f>
         <v>2.4300000000000002</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.62</v>
       </c>
       <c r="D7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.4300000000000002</v>
       </c>
       <c r="E7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.81</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H7" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-0.81</v>
       </c>
       <c r="I7" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.81</v>
       </c>
       <c r="J7" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.4300000000000002</v>
       </c>
       <c r="K7" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2150000000000001</v>
       </c>
       <c r="L7" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="M7" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O7" s="8">
-        <f t="shared" si="10"/>
-        <v>2.83</v>
+        <f t="shared" si="11"/>
+        <v>2.4300000000000002</v>
       </c>
       <c r="P7" s="8">
-        <f t="shared" si="11"/>
-        <v>1.9649999999999999</v>
+        <f t="shared" si="12"/>
+        <v>1.5649999999999999</v>
       </c>
       <c r="Q7" s="8">
-        <f t="shared" si="12"/>
-        <v>2.83</v>
+        <f t="shared" si="13"/>
+        <v>2.4300000000000002</v>
       </c>
       <c r="R7" s="8">
-        <f t="shared" si="13"/>
-        <v>1.2650000000000001</v>
+        <f t="shared" si="14"/>
+        <v>0.8650000000000001</v>
       </c>
       <c r="T7">
         <v>1.4</v>
       </c>
       <c r="V7" s="8">
-        <f>(SQRT(POWER(Q7-O7,2)+POWER(R7-P7,2)))</f>
-        <v>0.69999999999999973</v>
+        <f t="shared" si="0"/>
+        <v>0.69999999999999984</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">
@@ -1098,71 +1117,71 @@
         <v>106</v>
       </c>
       <c r="B8">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2.4300000000000002</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.81</v>
       </c>
       <c r="D8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.4300000000000002</v>
       </c>
       <c r="E8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H8" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-0.81</v>
       </c>
       <c r="I8" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.81</v>
       </c>
       <c r="J8" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.4300000000000002</v>
       </c>
       <c r="K8" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.40500000000000003</v>
       </c>
       <c r="L8" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="M8" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O8" s="8">
-        <f t="shared" si="10"/>
-        <v>2.83</v>
+        <f t="shared" si="11"/>
+        <v>2.4300000000000002</v>
       </c>
       <c r="P8" s="8">
-        <f t="shared" si="11"/>
-        <v>1.155</v>
+        <f t="shared" si="12"/>
+        <v>0.755</v>
       </c>
       <c r="Q8" s="8">
-        <f t="shared" si="12"/>
-        <v>2.83</v>
+        <f t="shared" si="13"/>
+        <v>2.4300000000000002</v>
       </c>
       <c r="R8" s="8">
-        <f t="shared" si="13"/>
-        <v>0.45500000000000007</v>
+        <f t="shared" si="14"/>
+        <v>5.5000000000000049E-2</v>
       </c>
       <c r="T8">
         <v>1.4</v>
       </c>
       <c r="V8" s="8">
-        <f>(SQRT(POWER(Q8-O8,2)+POWER(R8-P8,2)))</f>
+        <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
     </row>
@@ -1179,63 +1198,63 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.4300000000000002</v>
       </c>
       <c r="E9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-0.81000700000000003</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H9" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-0.81000700000000003</v>
       </c>
       <c r="I9" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.81000700000000003</v>
       </c>
       <c r="J9" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.4300000000000002</v>
       </c>
       <c r="K9" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-0.40500350000000002</v>
       </c>
       <c r="L9" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="M9" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O9" s="8">
-        <f t="shared" si="10"/>
-        <v>2.83</v>
+        <f t="shared" si="11"/>
+        <v>2.4300000000000002</v>
       </c>
       <c r="P9" s="8">
-        <f t="shared" si="11"/>
-        <v>0.34499649999999998</v>
+        <f t="shared" si="12"/>
+        <v>-5.5003500000000038E-2</v>
       </c>
       <c r="Q9" s="8">
-        <f t="shared" si="12"/>
-        <v>2.83</v>
+        <f t="shared" si="13"/>
+        <v>2.4300000000000002</v>
       </c>
       <c r="R9" s="8">
-        <f t="shared" si="13"/>
-        <v>-0.35500349999999992</v>
+        <f t="shared" si="14"/>
+        <v>-0.75500349999999994</v>
       </c>
       <c r="T9">
         <v>1.4</v>
       </c>
       <c r="V9" s="8">
-        <f>(SQRT(POWER(Q9-O9,2)+POWER(R9-P9,2)))</f>
+        <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
     </row>
@@ -1244,72 +1263,72 @@
         <v>108</v>
       </c>
       <c r="B10">
-        <f t="shared" ref="B10:B14" si="15">B22 * -1</f>
+        <f t="shared" ref="B10:B14" si="16">B22 * -1</f>
         <v>2.4300000000000002</v>
       </c>
       <c r="C10">
-        <f t="shared" ref="C10:C20" si="16">C22*-1</f>
+        <f t="shared" ref="C10:C14" si="17">C22*-1</f>
         <v>-0.81000700000000003</v>
       </c>
       <c r="D10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.4300000000000002</v>
       </c>
       <c r="E10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-1.6200140000000001</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H10" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-0.81000700000000003</v>
       </c>
       <c r="I10" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.81000700000000003</v>
       </c>
       <c r="J10" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.4300000000000002</v>
       </c>
       <c r="K10" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-1.2150105</v>
       </c>
       <c r="L10" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="M10" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O10" s="8">
-        <f t="shared" si="10"/>
-        <v>2.83</v>
+        <f t="shared" si="11"/>
+        <v>2.4300000000000002</v>
       </c>
       <c r="P10" s="8">
-        <f t="shared" si="11"/>
-        <v>-0.46501049999999999</v>
+        <f t="shared" si="12"/>
+        <v>-0.86501050000000002</v>
       </c>
       <c r="Q10" s="8">
-        <f t="shared" si="12"/>
-        <v>2.83</v>
+        <f t="shared" si="13"/>
+        <v>2.4300000000000002</v>
       </c>
       <c r="R10" s="8">
-        <f t="shared" si="13"/>
-        <v>-1.1650105000000002</v>
+        <f t="shared" si="14"/>
+        <v>-1.5650105000000001</v>
       </c>
       <c r="T10">
         <v>1.4</v>
       </c>
       <c r="V10" s="8">
-        <f>(SQRT(POWER(Q10-O10,2)+POWER(R10-P10,2)))</f>
-        <v>0.70000000000000018</v>
+        <f t="shared" si="0"/>
+        <v>0.70000000000000007</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
@@ -1317,71 +1336,71 @@
         <v>109</v>
       </c>
       <c r="B11">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2.4300000000000002</v>
       </c>
       <c r="C11">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-1.6200140000000001</v>
       </c>
       <c r="D11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.025007</v>
       </c>
       <c r="E11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-2.321507</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.40499300000000016</v>
       </c>
       <c r="H11" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-0.70149299999999992</v>
       </c>
       <c r="I11" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.8100072586699455</v>
       </c>
       <c r="J11" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.2275035000000001</v>
       </c>
       <c r="K11" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-1.9707604999999999</v>
       </c>
       <c r="L11" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.86603297994127981</v>
       </c>
       <c r="M11" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.49998687748182646</v>
       </c>
       <c r="O11" s="8">
-        <f t="shared" si="10"/>
-        <v>2.8024989071186392</v>
+        <f t="shared" si="11"/>
+        <v>2.4024989071186393</v>
       </c>
       <c r="P11" s="8">
-        <f t="shared" si="11"/>
-        <v>-1.267648957020552</v>
+        <f t="shared" si="12"/>
+        <v>-1.6676489570205519</v>
       </c>
       <c r="Q11" s="8">
-        <f t="shared" si="12"/>
-        <v>2.4525080928813607</v>
+        <f t="shared" si="13"/>
+        <v>2.0525080928813608</v>
       </c>
       <c r="R11" s="8">
-        <f t="shared" si="13"/>
-        <v>-1.873872042979448</v>
+        <f t="shared" si="14"/>
+        <v>-2.2738720429794479</v>
       </c>
       <c r="T11">
         <v>1.4</v>
       </c>
       <c r="V11" s="8">
-        <f>(SQRT(POWER(Q11-O11,2)+POWER(R11-P11,2)))</f>
+        <f t="shared" si="0"/>
         <v>0.70000000000000007</v>
       </c>
     </row>
@@ -1390,71 +1409,71 @@
         <v>110</v>
       </c>
       <c r="B12">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2.025007</v>
       </c>
       <c r="C12">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-2.321507</v>
       </c>
       <c r="D12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.6200140000000001</v>
       </c>
       <c r="E12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.0230000000000001</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.40499299999999994</v>
       </c>
       <c r="H12" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-0.70149300000000014</v>
       </c>
       <c r="I12" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.81000725866994561</v>
       </c>
       <c r="J12" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.8225104999999999</v>
       </c>
       <c r="K12" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-2.6722535000000001</v>
       </c>
       <c r="L12" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.86603297994127992</v>
       </c>
       <c r="M12" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.49998687748182613</v>
       </c>
       <c r="O12" s="8">
-        <f t="shared" si="10"/>
-        <v>2.3975059071186391</v>
+        <f t="shared" si="11"/>
+        <v>1.9975059071186392</v>
       </c>
       <c r="P12" s="8">
-        <f t="shared" si="11"/>
-        <v>-1.9691419570205522</v>
+        <f t="shared" si="12"/>
+        <v>-2.3691419570205521</v>
       </c>
       <c r="Q12" s="8">
-        <f t="shared" si="12"/>
-        <v>2.0475150928813606</v>
+        <f t="shared" si="13"/>
+        <v>1.6475150928813607</v>
       </c>
       <c r="R12" s="8">
-        <f t="shared" si="13"/>
-        <v>-2.5753650429794481</v>
+        <f t="shared" si="14"/>
+        <v>-2.975365042979448</v>
       </c>
       <c r="T12">
         <v>1.4</v>
       </c>
       <c r="V12" s="8">
-        <f>(SQRT(POWER(Q12-O12,2)+POWER(R12-P12,2)))</f>
+        <f t="shared" si="0"/>
         <v>0.70000000000000007</v>
       </c>
     </row>
@@ -1463,72 +1482,72 @@
         <v>111</v>
       </c>
       <c r="B13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.6200140000000001</v>
       </c>
       <c r="C13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-3.0230000000000001</v>
       </c>
       <c r="D13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.81000700000000003</v>
       </c>
       <c r="E13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.0230000000000001</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.81000700000000003</v>
       </c>
       <c r="H13" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I13" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.81000700000000003</v>
       </c>
       <c r="J13" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.2150105</v>
       </c>
       <c r="K13" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-3.0230000000000001</v>
       </c>
       <c r="L13" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M13" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="O13" s="8">
-        <f t="shared" si="10"/>
-        <v>1.9650105</v>
+        <f t="shared" si="11"/>
+        <v>1.5650105000000001</v>
       </c>
       <c r="P13" s="8">
-        <f t="shared" si="11"/>
-        <v>-2.6230000000000002</v>
+        <f t="shared" si="12"/>
+        <v>-3.0230000000000001</v>
       </c>
       <c r="Q13" s="8">
-        <f t="shared" si="12"/>
-        <v>1.2650105</v>
+        <f t="shared" si="13"/>
+        <v>0.86501050000000002</v>
       </c>
       <c r="R13" s="8">
-        <f t="shared" si="13"/>
-        <v>-2.6230000000000002</v>
+        <f t="shared" si="14"/>
+        <v>-3.0230000000000001</v>
       </c>
       <c r="T13">
         <v>1.4</v>
       </c>
       <c r="V13" s="8">
-        <f>(SQRT(POWER(Q13-O13,2)+POWER(R13-P13,2)))</f>
-        <v>0.7</v>
+        <f t="shared" si="0"/>
+        <v>0.70000000000000007</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.2">
@@ -1536,72 +1555,72 @@
         <v>112</v>
       </c>
       <c r="B14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.81000700000000003</v>
       </c>
       <c r="C14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-3.0230000000000001</v>
       </c>
       <c r="D14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.0230000000000001</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.81000700000000003</v>
       </c>
       <c r="H14" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I14" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.81000700000000003</v>
       </c>
       <c r="J14" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.40500350000000002</v>
       </c>
       <c r="K14" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-3.0230000000000001</v>
       </c>
       <c r="L14" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M14" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="O14" s="8">
-        <f t="shared" si="10"/>
-        <v>1.1550034999999998</v>
+        <f t="shared" si="11"/>
+        <v>0.75500349999999994</v>
       </c>
       <c r="P14" s="8">
-        <f t="shared" si="11"/>
-        <v>-2.6230000000000002</v>
+        <f t="shared" si="12"/>
+        <v>-3.0230000000000001</v>
       </c>
       <c r="Q14" s="8">
-        <f t="shared" si="12"/>
-        <v>0.45500350000000006</v>
+        <f t="shared" si="13"/>
+        <v>5.5003500000000038E-2</v>
       </c>
       <c r="R14" s="8">
-        <f t="shared" si="13"/>
-        <v>-2.6230000000000002</v>
+        <f t="shared" si="14"/>
+        <v>-3.0230000000000001</v>
       </c>
       <c r="T14">
         <v>1.4</v>
       </c>
       <c r="V14" s="8">
-        <f>(SQRT(POWER(Q14-O14,2)+POWER(R14-P14,2)))</f>
-        <v>0.69999999999999973</v>
+        <f t="shared" si="0"/>
+        <v>0.7</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
@@ -1616,63 +1635,63 @@
         <v>-3.0230000000000001</v>
       </c>
       <c r="D15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.81</v>
       </c>
       <c r="E15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.0230000000000001</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.81</v>
       </c>
       <c r="H15" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I15" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.81</v>
       </c>
       <c r="J15" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-0.40500000000000003</v>
       </c>
       <c r="K15" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-3.0230000000000001</v>
       </c>
       <c r="L15" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M15" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="O15" s="8">
-        <f t="shared" si="10"/>
-        <v>0.34499999999999997</v>
+        <f t="shared" si="11"/>
+        <v>-5.5000000000000049E-2</v>
       </c>
       <c r="P15" s="8">
-        <f t="shared" si="11"/>
-        <v>-2.6230000000000002</v>
+        <f t="shared" si="12"/>
+        <v>-3.0230000000000001</v>
       </c>
       <c r="Q15" s="8">
-        <f t="shared" si="12"/>
-        <v>-0.35499999999999998</v>
+        <f t="shared" si="13"/>
+        <v>-0.755</v>
       </c>
       <c r="R15" s="8">
-        <f t="shared" si="13"/>
-        <v>-2.6230000000000002</v>
+        <f t="shared" si="14"/>
+        <v>-3.0230000000000001</v>
       </c>
       <c r="T15">
         <v>1.4</v>
       </c>
       <c r="V15" s="8">
-        <f>(SQRT(POWER(Q15-O15,2)+POWER(R15-P15,2)))</f>
+        <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
     </row>
@@ -1685,68 +1704,68 @@
         <v>-0.81</v>
       </c>
       <c r="C16">
-        <f t="shared" ref="C16:C20" si="17">C27* -1</f>
+        <f t="shared" ref="C16:C20" si="18">C27* -1</f>
         <v>-3.0230000000000001</v>
       </c>
       <c r="D16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.62</v>
       </c>
       <c r="E16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.0230000000000001</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.81</v>
       </c>
       <c r="H16" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I16" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.81</v>
       </c>
       <c r="J16" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-1.2150000000000001</v>
       </c>
       <c r="K16" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-3.0230000000000001</v>
       </c>
       <c r="L16" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M16" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="O16" s="8">
-        <f t="shared" si="10"/>
-        <v>-0.46500000000000008</v>
+        <f t="shared" si="11"/>
+        <v>-0.8650000000000001</v>
       </c>
       <c r="P16" s="8">
-        <f t="shared" si="11"/>
-        <v>-2.6230000000000002</v>
+        <f t="shared" si="12"/>
+        <v>-3.0230000000000001</v>
       </c>
       <c r="Q16" s="8">
-        <f t="shared" si="12"/>
-        <v>-1.165</v>
+        <f t="shared" si="13"/>
+        <v>-1.5649999999999999</v>
       </c>
       <c r="R16" s="8">
-        <f t="shared" si="13"/>
-        <v>-2.6230000000000002</v>
+        <f t="shared" si="14"/>
+        <v>-3.0230000000000001</v>
       </c>
       <c r="T16">
         <v>1.4</v>
       </c>
       <c r="V16" s="8">
-        <f>(SQRT(POWER(Q16-O16,2)+POWER(R16-P16,2)))</f>
-        <v>0.7</v>
+        <f t="shared" si="0"/>
+        <v>0.69999999999999984</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.2">
@@ -1754,71 +1773,71 @@
         <v>203</v>
       </c>
       <c r="B17">
-        <f t="shared" ref="B17:B20" si="18">B28</f>
+        <f t="shared" ref="B17:B20" si="19">B28</f>
         <v>-1.62</v>
       </c>
       <c r="C17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-3.0230000000000001</v>
       </c>
       <c r="D17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-2.0249999999999999</v>
       </c>
       <c r="E17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-2.3214999999999999</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.4049999999999998</v>
       </c>
       <c r="H17" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.70150000000000023</v>
       </c>
       <c r="I17" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.8100168208130003</v>
       </c>
       <c r="J17" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-1.8225</v>
       </c>
       <c r="K17" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-2.67225</v>
       </c>
       <c r="L17" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.86603139833061304</v>
       </c>
       <c r="M17" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.49998961699771627</v>
       </c>
       <c r="O17" s="8">
-        <f t="shared" si="10"/>
-        <v>-1.2475036340507994</v>
+        <f t="shared" si="11"/>
+        <v>-1.6475036340507994</v>
       </c>
       <c r="P17" s="8">
-        <f t="shared" si="11"/>
-        <v>-2.5753609894157146</v>
+        <f t="shared" si="12"/>
+        <v>-2.9753609894157145</v>
       </c>
       <c r="Q17" s="8">
-        <f t="shared" si="12"/>
-        <v>-1.5974963659492007</v>
+        <f t="shared" si="13"/>
+        <v>-1.9974963659492007</v>
       </c>
       <c r="R17" s="8">
-        <f t="shared" si="13"/>
-        <v>-1.9691390105842856</v>
+        <f t="shared" si="14"/>
+        <v>-2.3691390105842856</v>
       </c>
       <c r="T17">
         <v>1.4</v>
       </c>
       <c r="V17" s="8">
-        <f>(SQRT(POWER(Q17-O17,2)+POWER(R17-P17,2)))</f>
+        <f t="shared" si="0"/>
         <v>0.69999999999999973</v>
       </c>
     </row>
@@ -1827,72 +1846,72 @@
         <v>204</v>
       </c>
       <c r="B18">
+        <f t="shared" si="19"/>
+        <v>-2.0249999999999999</v>
+      </c>
+      <c r="C18">
         <f t="shared" si="18"/>
-        <v>-2.0249999999999999</v>
-      </c>
-      <c r="C18">
-        <f t="shared" si="17"/>
         <v>-2.3214999999999999</v>
       </c>
       <c r="D18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-2.4300000000000002</v>
       </c>
       <c r="E18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-1.62</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.40500000000000025</v>
       </c>
       <c r="H18" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.70149999999999979</v>
       </c>
       <c r="I18" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.81001682081300008</v>
       </c>
       <c r="J18" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-2.2275</v>
       </c>
       <c r="K18" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-1.97075</v>
       </c>
       <c r="L18" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.86603139833061271</v>
       </c>
       <c r="M18" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.49998961699771699</v>
       </c>
       <c r="O18" s="8">
-        <f t="shared" si="10"/>
-        <v>-1.6525036340507993</v>
+        <f t="shared" si="11"/>
+        <v>-2.0525036340507992</v>
       </c>
       <c r="P18" s="8">
-        <f t="shared" si="11"/>
-        <v>-1.8738609894157143</v>
+        <f t="shared" si="12"/>
+        <v>-2.2738609894157142</v>
       </c>
       <c r="Q18" s="8">
-        <f t="shared" si="12"/>
-        <v>-2.002496365949201</v>
+        <f t="shared" si="13"/>
+        <v>-2.4024963659492009</v>
       </c>
       <c r="R18" s="8">
-        <f t="shared" si="13"/>
-        <v>-1.2676390105842854</v>
+        <f t="shared" si="14"/>
+        <v>-1.6676390105842855</v>
       </c>
       <c r="T18">
         <v>1.4</v>
       </c>
       <c r="V18" s="8">
-        <f>(SQRT(POWER(Q18-O18,2)+POWER(R18-P18,2)))</f>
-        <v>0.7</v>
+        <f t="shared" si="0"/>
+        <v>0.69999999999999984</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.2">
@@ -1900,72 +1919,72 @@
         <v>205</v>
       </c>
       <c r="B19">
+        <f t="shared" si="19"/>
+        <v>-2.4300000000000002</v>
+      </c>
+      <c r="C19">
         <f t="shared" si="18"/>
+        <v>-1.62</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="2"/>
         <v>-2.4300000000000002</v>
       </c>
-      <c r="C19">
-        <f t="shared" si="17"/>
-        <v>-1.62</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="1"/>
-        <v>-2.4300000000000002</v>
-      </c>
       <c r="E19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-0.81</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H19" s="8">
-        <f t="shared" si="4"/>
-        <v>0.81</v>
-      </c>
-      <c r="I19" s="8">
         <f t="shared" si="5"/>
         <v>0.81</v>
       </c>
+      <c r="I19" s="8">
+        <f t="shared" si="6"/>
+        <v>0.81</v>
+      </c>
       <c r="J19" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-2.4300000000000002</v>
       </c>
       <c r="K19" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-1.2150000000000001</v>
       </c>
       <c r="L19" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="M19" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O19" s="8">
-        <f t="shared" si="10"/>
-        <v>-2.0300000000000002</v>
+        <f t="shared" si="11"/>
+        <v>-2.4300000000000002</v>
       </c>
       <c r="P19" s="8">
-        <f t="shared" si="11"/>
-        <v>-1.165</v>
+        <f t="shared" si="12"/>
+        <v>-1.5649999999999999</v>
       </c>
       <c r="Q19" s="8">
-        <f t="shared" si="12"/>
-        <v>-2.0300000000000002</v>
+        <f t="shared" si="13"/>
+        <v>-2.4300000000000002</v>
       </c>
       <c r="R19" s="8">
-        <f t="shared" si="13"/>
-        <v>-0.46500000000000008</v>
+        <f t="shared" si="14"/>
+        <v>-0.8650000000000001</v>
       </c>
       <c r="T19">
         <v>1.4</v>
       </c>
       <c r="V19" s="8">
-        <f>(SQRT(POWER(Q19-O19,2)+POWER(R19-P19,2)))</f>
-        <v>0.7</v>
+        <f t="shared" si="0"/>
+        <v>0.69999999999999984</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.2">
@@ -1973,71 +1992,71 @@
         <v>206</v>
       </c>
       <c r="B20">
+        <f t="shared" si="19"/>
+        <v>-2.4300000000000002</v>
+      </c>
+      <c r="C20">
         <f t="shared" si="18"/>
+        <v>-0.81</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="2"/>
         <v>-2.4300000000000002</v>
       </c>
-      <c r="C20">
-        <f t="shared" si="17"/>
-        <v>-0.81</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="1"/>
-        <v>-2.4300000000000002</v>
-      </c>
       <c r="E20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H20" s="8">
-        <f t="shared" si="4"/>
-        <v>0.81</v>
-      </c>
-      <c r="I20" s="8">
         <f t="shared" si="5"/>
         <v>0.81</v>
       </c>
+      <c r="I20" s="8">
+        <f t="shared" si="6"/>
+        <v>0.81</v>
+      </c>
       <c r="J20" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-2.4300000000000002</v>
       </c>
       <c r="K20" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-0.40500000000000003</v>
       </c>
       <c r="L20" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="M20" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O20" s="8">
-        <f t="shared" si="10"/>
-        <v>-2.0300000000000002</v>
+        <f t="shared" si="11"/>
+        <v>-2.4300000000000002</v>
       </c>
       <c r="P20" s="8">
-        <f t="shared" si="11"/>
-        <v>-0.35499999999999998</v>
+        <f t="shared" si="12"/>
+        <v>-0.755</v>
       </c>
       <c r="Q20" s="8">
-        <f t="shared" si="12"/>
-        <v>-2.0300000000000002</v>
+        <f t="shared" si="13"/>
+        <v>-2.4300000000000002</v>
       </c>
       <c r="R20" s="8">
-        <f t="shared" si="13"/>
-        <v>0.34499999999999997</v>
+        <f t="shared" si="14"/>
+        <v>-5.5000000000000049E-2</v>
       </c>
       <c r="T20">
         <v>1.4</v>
       </c>
       <c r="V20" s="8">
-        <f>(SQRT(POWER(Q20-O20,2)+POWER(R20-P20,2)))</f>
+        <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
     </row>
@@ -2052,64 +2071,64 @@
         <v>0</v>
       </c>
       <c r="D21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-2.4300000000000002</v>
       </c>
       <c r="E21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.81000700000000003</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H21" s="8">
-        <f t="shared" si="4"/>
-        <v>0.81000700000000003</v>
-      </c>
-      <c r="I21" s="8">
         <f t="shared" si="5"/>
         <v>0.81000700000000003</v>
       </c>
+      <c r="I21" s="8">
+        <f t="shared" si="6"/>
+        <v>0.81000700000000003</v>
+      </c>
       <c r="J21" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-2.4300000000000002</v>
       </c>
       <c r="K21" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.40500350000000002</v>
       </c>
       <c r="L21" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="M21" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O21" s="8">
-        <f t="shared" si="10"/>
-        <v>-2.0300000000000002</v>
+        <f t="shared" si="11"/>
+        <v>-2.4300000000000002</v>
       </c>
       <c r="P21" s="8">
-        <f t="shared" si="11"/>
-        <v>0.45500350000000006</v>
+        <f t="shared" si="12"/>
+        <v>5.5003500000000038E-2</v>
       </c>
       <c r="Q21" s="8">
-        <f t="shared" si="12"/>
-        <v>-2.0300000000000002</v>
+        <f t="shared" si="13"/>
+        <v>-2.4300000000000002</v>
       </c>
       <c r="R21" s="8">
-        <f t="shared" si="13"/>
-        <v>1.1550034999999998</v>
+        <f t="shared" si="14"/>
+        <v>0.75500349999999994</v>
       </c>
       <c r="T21">
         <v>1.4</v>
       </c>
       <c r="V21" s="8">
-        <f>(SQRT(POWER(Q21-O21,2)+POWER(R21-P21,2)))</f>
-        <v>0.69999999999999973</v>
+        <f t="shared" si="0"/>
+        <v>0.7</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.2">
@@ -2123,64 +2142,64 @@
         <v>0.81000700000000003</v>
       </c>
       <c r="D22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-2.4300000000000002</v>
       </c>
       <c r="E22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.6200140000000001</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H22" s="8">
-        <f t="shared" si="4"/>
-        <v>0.81000700000000003</v>
-      </c>
-      <c r="I22" s="8">
         <f t="shared" si="5"/>
         <v>0.81000700000000003</v>
       </c>
+      <c r="I22" s="8">
+        <f t="shared" si="6"/>
+        <v>0.81000700000000003</v>
+      </c>
       <c r="J22" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-2.4300000000000002</v>
       </c>
       <c r="K22" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2150105</v>
       </c>
       <c r="L22" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="M22" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O22" s="8">
-        <f t="shared" si="10"/>
-        <v>-2.0300000000000002</v>
+        <f t="shared" si="11"/>
+        <v>-2.4300000000000002</v>
       </c>
       <c r="P22" s="8">
-        <f t="shared" si="11"/>
-        <v>1.2650105</v>
+        <f t="shared" si="12"/>
+        <v>0.86501050000000002</v>
       </c>
       <c r="Q22" s="8">
-        <f t="shared" si="12"/>
-        <v>-2.0300000000000002</v>
+        <f t="shared" si="13"/>
+        <v>-2.4300000000000002</v>
       </c>
       <c r="R22" s="8">
-        <f t="shared" si="13"/>
-        <v>1.9650105</v>
+        <f t="shared" si="14"/>
+        <v>1.5650105000000001</v>
       </c>
       <c r="T22">
         <v>1.4</v>
       </c>
       <c r="V22" s="8">
-        <f>(SQRT(POWER(Q22-O22,2)+POWER(R22-P22,2)))</f>
-        <v>0.7</v>
+        <f t="shared" si="0"/>
+        <v>0.70000000000000007</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.2">
@@ -2194,63 +2213,63 @@
         <v>1.6200140000000001</v>
       </c>
       <c r="D23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-2.025007</v>
       </c>
       <c r="E23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.321507</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.40499300000000016</v>
       </c>
       <c r="H23" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.70149299999999992</v>
       </c>
       <c r="I23" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.8100072586699455</v>
       </c>
       <c r="J23" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-2.2275035000000001</v>
       </c>
       <c r="K23" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.9707604999999999</v>
       </c>
       <c r="L23" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.86603297994127981</v>
       </c>
       <c r="M23" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-0.49998687748182646</v>
       </c>
       <c r="O23" s="8">
-        <f t="shared" si="10"/>
-        <v>-2.0024989071186394</v>
+        <f t="shared" si="11"/>
+        <v>-2.4024989071186393</v>
       </c>
       <c r="P23" s="8">
-        <f t="shared" si="11"/>
-        <v>2.0676489570205518</v>
+        <f t="shared" si="12"/>
+        <v>1.6676489570205519</v>
       </c>
       <c r="Q23" s="8">
-        <f t="shared" si="12"/>
-        <v>-1.6525080928813609</v>
+        <f t="shared" si="13"/>
+        <v>-2.0525080928813608</v>
       </c>
       <c r="R23" s="8">
-        <f t="shared" si="13"/>
-        <v>2.6738720429794478</v>
+        <f t="shared" si="14"/>
+        <v>2.2738720429794479</v>
       </c>
       <c r="T23">
         <v>1.4</v>
       </c>
       <c r="V23" s="8">
-        <f>(SQRT(POWER(Q23-O23,2)+POWER(R23-P23,2)))</f>
+        <f t="shared" si="0"/>
         <v>0.70000000000000007</v>
       </c>
     </row>
@@ -2265,63 +2284,63 @@
         <v>2.321507</v>
       </c>
       <c r="D24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.6200140000000001</v>
       </c>
       <c r="E24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.0230000000000001</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.40499299999999994</v>
       </c>
       <c r="H24" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.70149300000000014</v>
       </c>
       <c r="I24" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.81000725866994561</v>
       </c>
       <c r="J24" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-1.8225104999999999</v>
       </c>
       <c r="K24" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.6722535000000001</v>
       </c>
       <c r="L24" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.86603297994127992</v>
       </c>
       <c r="M24" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-0.49998687748182613</v>
       </c>
       <c r="O24" s="8">
-        <f t="shared" si="10"/>
-        <v>-1.5975059071186393</v>
+        <f t="shared" si="11"/>
+        <v>-1.9975059071186392</v>
       </c>
       <c r="P24" s="8">
-        <f t="shared" si="11"/>
-        <v>2.769141957020552</v>
+        <f t="shared" si="12"/>
+        <v>2.3691419570205521</v>
       </c>
       <c r="Q24" s="8">
-        <f t="shared" si="12"/>
-        <v>-1.2475150928813608</v>
+        <f t="shared" si="13"/>
+        <v>-1.6475150928813607</v>
       </c>
       <c r="R24" s="8">
-        <f t="shared" si="13"/>
-        <v>3.3753650429794479</v>
+        <f t="shared" si="14"/>
+        <v>2.975365042979448</v>
       </c>
       <c r="T24">
         <v>1.4</v>
       </c>
       <c r="V24" s="8">
-        <f>(SQRT(POWER(Q24-O24,2)+POWER(R24-P24,2)))</f>
+        <f t="shared" si="0"/>
         <v>0.70000000000000007</v>
       </c>
     </row>
@@ -2336,64 +2355,64 @@
         <v>3.0230000000000001</v>
       </c>
       <c r="D25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.81000700000000003</v>
       </c>
       <c r="E25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.0230000000000001</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.81000700000000003</v>
       </c>
       <c r="H25" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I25" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.81000700000000003</v>
       </c>
       <c r="J25" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-1.2150105</v>
       </c>
       <c r="K25" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.0230000000000001</v>
       </c>
       <c r="L25" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M25" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-1</v>
       </c>
       <c r="O25" s="8">
-        <f t="shared" si="10"/>
-        <v>-1.1650105000000002</v>
+        <f t="shared" si="11"/>
+        <v>-1.5650105000000001</v>
       </c>
       <c r="P25" s="8">
-        <f t="shared" si="11"/>
-        <v>3.423</v>
+        <f t="shared" si="12"/>
+        <v>3.0230000000000001</v>
       </c>
       <c r="Q25" s="8">
-        <f t="shared" si="12"/>
-        <v>-0.46501049999999999</v>
+        <f t="shared" si="13"/>
+        <v>-0.86501050000000002</v>
       </c>
       <c r="R25" s="8">
-        <f t="shared" si="13"/>
-        <v>3.423</v>
+        <f t="shared" si="14"/>
+        <v>3.0230000000000001</v>
       </c>
       <c r="T25">
         <v>1.4</v>
       </c>
       <c r="V25" s="8">
-        <f>(SQRT(POWER(Q25-O25,2)+POWER(R25-P25,2)))</f>
-        <v>0.70000000000000018</v>
+        <f t="shared" si="0"/>
+        <v>0.70000000000000007</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.2">
@@ -2414,54 +2433,54 @@
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.81000700000000003</v>
       </c>
       <c r="H26" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I26" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.81000700000000003</v>
       </c>
       <c r="J26" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-0.40500350000000002</v>
       </c>
       <c r="K26" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.0230000000000001</v>
       </c>
       <c r="L26" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M26" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-1</v>
       </c>
       <c r="O26" s="8">
-        <f t="shared" si="10"/>
-        <v>-0.35500349999999992</v>
+        <f t="shared" si="11"/>
+        <v>-0.75500349999999994</v>
       </c>
       <c r="P26" s="8">
-        <f t="shared" si="11"/>
-        <v>3.423</v>
+        <f t="shared" si="12"/>
+        <v>3.0230000000000001</v>
       </c>
       <c r="Q26" s="8">
-        <f t="shared" si="12"/>
-        <v>0.34499649999999998</v>
+        <f t="shared" si="13"/>
+        <v>-5.5003500000000038E-2</v>
       </c>
       <c r="R26" s="8">
-        <f t="shared" si="13"/>
-        <v>3.423</v>
+        <f t="shared" si="14"/>
+        <v>3.0230000000000001</v>
       </c>
       <c r="T26">
         <v>1.4</v>
       </c>
       <c r="V26" s="8">
-        <f>(SQRT(POWER(Q26-O26,2)+POWER(R26-P26,2)))</f>
+        <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
     </row>
@@ -2511,15 +2530,15 @@
       <c r="C30" s="2">
         <v>1.62</v>
       </c>
-      <c r="G30" s="10" t="s">
+      <c r="G30" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="12" t="s">
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="K30" s="13" t="s">
+      <c r="K30" s="12" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2533,15 +2552,15 @@
       <c r="C31" s="2">
         <v>0.81</v>
       </c>
-      <c r="G31" s="14">
+      <c r="G31" s="13">
         <v>0.7</v>
       </c>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
-      <c r="J31" s="15">
-        <v>0.4</v>
-      </c>
-      <c r="K31" s="16">
+      <c r="J31" s="14">
+        <v>0</v>
+      </c>
+      <c r="K31" s="15">
         <v>0</v>
       </c>
     </row>
@@ -2554,16 +2573,198 @@
       </c>
       <c r="C32" s="2">
         <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="E35" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F35" s="16"/>
+    </row>
+    <row r="36" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37">
+        <f>B25</f>
+        <v>-1.6200140000000001</v>
+      </c>
+      <c r="C37">
+        <f>C25</f>
+        <v>3.0230000000000001</v>
+      </c>
+      <c r="E37">
+        <f>B37+$J$31</f>
+        <v>-1.6200140000000001</v>
+      </c>
+      <c r="F37">
+        <f>C37 + $K$31</f>
+        <v>3.0230000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>2</v>
+      </c>
+      <c r="B38">
+        <f>D4</f>
+        <v>1.62</v>
+      </c>
+      <c r="C38">
+        <f>E4</f>
+        <v>3.0230000000000001</v>
+      </c>
+      <c r="E38">
+        <f t="shared" ref="E38:E43" si="20">B38+$J$31</f>
+        <v>1.62</v>
+      </c>
+      <c r="F38">
+        <f t="shared" ref="F38:F43" si="21">C38 + $K$31</f>
+        <v>3.0230000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>3</v>
+      </c>
+      <c r="B39">
+        <f>D6</f>
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="C39">
+        <f>E6</f>
+        <v>1.62</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="20"/>
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="21"/>
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>4</v>
+      </c>
+      <c r="B40">
+        <f>D10</f>
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="C40">
+        <f>E10</f>
+        <v>-1.6200140000000001</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="20"/>
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="21"/>
+        <v>-1.6200140000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>5</v>
+      </c>
+      <c r="B41">
+        <f>D12</f>
+        <v>1.6200140000000001</v>
+      </c>
+      <c r="C41">
+        <f>E12</f>
+        <v>-3.0230000000000001</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="20"/>
+        <v>1.6200140000000001</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="21"/>
+        <v>-3.0230000000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>6</v>
+      </c>
+      <c r="B42">
+        <f>D16</f>
+        <v>-1.62</v>
+      </c>
+      <c r="C42">
+        <f>E16</f>
+        <v>-3.0230000000000001</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="20"/>
+        <v>-1.62</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="21"/>
+        <v>-3.0230000000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>7</v>
+      </c>
+      <c r="B43">
+        <f>D18</f>
+        <v>-2.4300000000000002</v>
+      </c>
+      <c r="C43">
+        <f>E18</f>
+        <v>-1.62</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="20"/>
+        <v>-2.4300000000000002</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="21"/>
+        <v>-1.62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A27:C32">
     <sortCondition descending="1" ref="A27:A32"/>
   </sortState>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="G1:M1"/>
     <mergeCell ref="O1:R1"/>
     <mergeCell ref="B1:E1"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="E35:F35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2609,19 +2810,19 @@
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
         <f>Sheet1!O3</f>
-        <v>0.45500000000000007</v>
+        <v>5.5000000000000049E-2</v>
       </c>
       <c r="B2" s="8">
         <f>Sheet1!P3</f>
-        <v>3.423</v>
+        <v>3.0230000000000001</v>
       </c>
       <c r="C2" s="8">
         <f>Sheet1!Q3</f>
-        <v>1.155</v>
+        <v>0.755</v>
       </c>
       <c r="D2" s="8">
         <f>Sheet1!R3</f>
-        <v>3.423</v>
+        <v>3.0230000000000001</v>
       </c>
       <c r="E2" s="8">
         <f>Sheet1!T3</f>
@@ -2639,19 +2840,19 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <f>Sheet1!O4</f>
-        <v>1.2650000000000001</v>
+        <v>0.8650000000000001</v>
       </c>
       <c r="B3" s="8">
         <f>Sheet1!P4</f>
-        <v>3.423</v>
+        <v>3.0230000000000001</v>
       </c>
       <c r="C3" s="8">
         <f>Sheet1!Q4</f>
-        <v>1.9649999999999999</v>
+        <v>1.5649999999999999</v>
       </c>
       <c r="D3" s="8">
         <f>Sheet1!R4</f>
-        <v>3.423</v>
+        <v>3.0230000000000001</v>
       </c>
       <c r="E3" s="8">
         <f>Sheet1!T4</f>
@@ -2669,19 +2870,19 @@
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
         <f>Sheet1!O5</f>
-        <v>2.0475036340507993</v>
+        <v>1.6475036340507994</v>
       </c>
       <c r="B4" s="8">
         <f>Sheet1!P5</f>
-        <v>3.3753609894157144</v>
+        <v>2.9753609894157145</v>
       </c>
       <c r="C4" s="8">
         <f>Sheet1!Q5</f>
-        <v>2.3974963659492006</v>
+        <v>1.9974963659492007</v>
       </c>
       <c r="D4" s="8">
         <f>Sheet1!R5</f>
-        <v>2.7691390105842855</v>
+        <v>2.3691390105842856</v>
       </c>
       <c r="E4" s="8">
         <f>Sheet1!T5</f>
@@ -2699,19 +2900,19 @@
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <f>Sheet1!O6</f>
-        <v>2.4525036340507991</v>
+        <v>2.0525036340507992</v>
       </c>
       <c r="B5" s="8">
         <f>Sheet1!P6</f>
-        <v>2.6738609894157142</v>
+        <v>2.2738609894157142</v>
       </c>
       <c r="C5" s="8">
         <f>Sheet1!Q6</f>
-        <v>2.8024963659492008</v>
+        <v>2.4024963659492009</v>
       </c>
       <c r="D5" s="8">
         <f>Sheet1!R6</f>
-        <v>2.0676390105842857</v>
+        <v>1.6676390105842855</v>
       </c>
       <c r="E5" s="8">
         <f>Sheet1!T6</f>
@@ -2729,19 +2930,19 @@
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <f>Sheet1!O7</f>
-        <v>2.83</v>
+        <v>2.4300000000000002</v>
       </c>
       <c r="B6" s="8">
         <f>Sheet1!P7</f>
-        <v>1.9649999999999999</v>
+        <v>1.5649999999999999</v>
       </c>
       <c r="C6" s="8">
         <f>Sheet1!Q7</f>
-        <v>2.83</v>
+        <v>2.4300000000000002</v>
       </c>
       <c r="D6" s="8">
         <f>Sheet1!R7</f>
-        <v>1.2650000000000001</v>
+        <v>0.8650000000000001</v>
       </c>
       <c r="E6" s="8">
         <f>Sheet1!T7</f>
@@ -2759,19 +2960,19 @@
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <f>Sheet1!O8</f>
-        <v>2.83</v>
+        <v>2.4300000000000002</v>
       </c>
       <c r="B7" s="8">
         <f>Sheet1!P8</f>
-        <v>1.155</v>
+        <v>0.755</v>
       </c>
       <c r="C7" s="8">
         <f>Sheet1!Q8</f>
-        <v>2.83</v>
+        <v>2.4300000000000002</v>
       </c>
       <c r="D7" s="8">
         <f>Sheet1!R8</f>
-        <v>0.45500000000000007</v>
+        <v>5.5000000000000049E-2</v>
       </c>
       <c r="E7" s="8">
         <f>Sheet1!T8</f>
@@ -2789,19 +2990,19 @@
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <f>Sheet1!O9</f>
-        <v>2.83</v>
+        <v>2.4300000000000002</v>
       </c>
       <c r="B8" s="8">
         <f>Sheet1!P9</f>
-        <v>0.34499649999999998</v>
+        <v>-5.5003500000000038E-2</v>
       </c>
       <c r="C8" s="8">
         <f>Sheet1!Q9</f>
-        <v>2.83</v>
+        <v>2.4300000000000002</v>
       </c>
       <c r="D8" s="8">
         <f>Sheet1!R9</f>
-        <v>-0.35500349999999992</v>
+        <v>-0.75500349999999994</v>
       </c>
       <c r="E8" s="8">
         <f>Sheet1!T9</f>
@@ -2819,19 +3020,19 @@
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <f>Sheet1!O10</f>
-        <v>2.83</v>
+        <v>2.4300000000000002</v>
       </c>
       <c r="B9" s="8">
         <f>Sheet1!P10</f>
-        <v>-0.46501049999999999</v>
+        <v>-0.86501050000000002</v>
       </c>
       <c r="C9" s="8">
         <f>Sheet1!Q10</f>
-        <v>2.83</v>
+        <v>2.4300000000000002</v>
       </c>
       <c r="D9" s="8">
         <f>Sheet1!R10</f>
-        <v>-1.1650105000000002</v>
+        <v>-1.5650105000000001</v>
       </c>
       <c r="E9" s="8">
         <f>Sheet1!T10</f>
@@ -2849,19 +3050,19 @@
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <f>Sheet1!O11</f>
-        <v>2.8024989071186392</v>
+        <v>2.4024989071186393</v>
       </c>
       <c r="B10" s="8">
         <f>Sheet1!P11</f>
-        <v>-1.267648957020552</v>
+        <v>-1.6676489570205519</v>
       </c>
       <c r="C10" s="8">
         <f>Sheet1!Q11</f>
-        <v>2.4525080928813607</v>
+        <v>2.0525080928813608</v>
       </c>
       <c r="D10" s="8">
         <f>Sheet1!R11</f>
-        <v>-1.873872042979448</v>
+        <v>-2.2738720429794479</v>
       </c>
       <c r="E10" s="8">
         <f>Sheet1!T11</f>
@@ -2879,19 +3080,19 @@
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
         <f>Sheet1!O12</f>
-        <v>2.3975059071186391</v>
+        <v>1.9975059071186392</v>
       </c>
       <c r="B11" s="8">
         <f>Sheet1!P12</f>
-        <v>-1.9691419570205522</v>
+        <v>-2.3691419570205521</v>
       </c>
       <c r="C11" s="8">
         <f>Sheet1!Q12</f>
-        <v>2.0475150928813606</v>
+        <v>1.6475150928813607</v>
       </c>
       <c r="D11" s="8">
         <f>Sheet1!R12</f>
-        <v>-2.5753650429794481</v>
+        <v>-2.975365042979448</v>
       </c>
       <c r="E11" s="8">
         <f>Sheet1!T12</f>
@@ -2909,19 +3110,19 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
         <f>Sheet1!O13</f>
-        <v>1.9650105</v>
+        <v>1.5650105000000001</v>
       </c>
       <c r="B12" s="8">
         <f>Sheet1!P13</f>
-        <v>-2.6230000000000002</v>
+        <v>-3.0230000000000001</v>
       </c>
       <c r="C12" s="8">
         <f>Sheet1!Q13</f>
-        <v>1.2650105</v>
+        <v>0.86501050000000002</v>
       </c>
       <c r="D12" s="8">
         <f>Sheet1!R13</f>
-        <v>-2.6230000000000002</v>
+        <v>-3.0230000000000001</v>
       </c>
       <c r="E12" s="8">
         <f>Sheet1!T13</f>
@@ -2939,19 +3140,19 @@
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="8">
         <f>Sheet1!O14</f>
-        <v>1.1550034999999998</v>
+        <v>0.75500349999999994</v>
       </c>
       <c r="B13" s="8">
         <f>Sheet1!P14</f>
-        <v>-2.6230000000000002</v>
+        <v>-3.0230000000000001</v>
       </c>
       <c r="C13" s="8">
         <f>Sheet1!Q14</f>
-        <v>0.45500350000000006</v>
+        <v>5.5003500000000038E-2</v>
       </c>
       <c r="D13" s="8">
         <f>Sheet1!R14</f>
-        <v>-2.6230000000000002</v>
+        <v>-3.0230000000000001</v>
       </c>
       <c r="E13" s="8">
         <f>Sheet1!T14</f>
@@ -2969,19 +3170,19 @@
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="8">
         <f>Sheet1!O15</f>
-        <v>0.34499999999999997</v>
+        <v>-5.5000000000000049E-2</v>
       </c>
       <c r="B14" s="8">
         <f>Sheet1!P15</f>
-        <v>-2.6230000000000002</v>
+        <v>-3.0230000000000001</v>
       </c>
       <c r="C14" s="8">
         <f>Sheet1!Q15</f>
-        <v>-0.35499999999999998</v>
+        <v>-0.755</v>
       </c>
       <c r="D14" s="8">
         <f>Sheet1!R15</f>
-        <v>-2.6230000000000002</v>
+        <v>-3.0230000000000001</v>
       </c>
       <c r="E14" s="8">
         <f>Sheet1!T15</f>
@@ -2999,19 +3200,19 @@
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="8">
         <f>Sheet1!O16</f>
-        <v>-0.46500000000000008</v>
+        <v>-0.8650000000000001</v>
       </c>
       <c r="B15" s="8">
         <f>Sheet1!P16</f>
-        <v>-2.6230000000000002</v>
+        <v>-3.0230000000000001</v>
       </c>
       <c r="C15" s="8">
         <f>Sheet1!Q16</f>
-        <v>-1.165</v>
+        <v>-1.5649999999999999</v>
       </c>
       <c r="D15" s="8">
         <f>Sheet1!R16</f>
-        <v>-2.6230000000000002</v>
+        <v>-3.0230000000000001</v>
       </c>
       <c r="E15" s="8">
         <f>Sheet1!T16</f>
@@ -3029,19 +3230,19 @@
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="8">
         <f>Sheet1!O17</f>
-        <v>-1.2475036340507994</v>
+        <v>-1.6475036340507994</v>
       </c>
       <c r="B16" s="8">
         <f>Sheet1!P17</f>
-        <v>-2.5753609894157146</v>
+        <v>-2.9753609894157145</v>
       </c>
       <c r="C16" s="8">
         <f>Sheet1!Q17</f>
-        <v>-1.5974963659492007</v>
+        <v>-1.9974963659492007</v>
       </c>
       <c r="D16" s="8">
         <f>Sheet1!R17</f>
-        <v>-1.9691390105842856</v>
+        <v>-2.3691390105842856</v>
       </c>
       <c r="E16" s="8">
         <f>Sheet1!T17</f>
@@ -3059,19 +3260,19 @@
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="8">
         <f>Sheet1!O18</f>
-        <v>-1.6525036340507993</v>
+        <v>-2.0525036340507992</v>
       </c>
       <c r="B17" s="8">
         <f>Sheet1!P18</f>
-        <v>-1.8738609894157143</v>
+        <v>-2.2738609894157142</v>
       </c>
       <c r="C17" s="8">
         <f>Sheet1!Q18</f>
-        <v>-2.002496365949201</v>
+        <v>-2.4024963659492009</v>
       </c>
       <c r="D17" s="8">
         <f>Sheet1!R18</f>
-        <v>-1.2676390105842854</v>
+        <v>-1.6676390105842855</v>
       </c>
       <c r="E17" s="8">
         <f>Sheet1!T18</f>
@@ -3089,19 +3290,19 @@
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="8">
         <f>Sheet1!O19</f>
-        <v>-2.0300000000000002</v>
+        <v>-2.4300000000000002</v>
       </c>
       <c r="B18" s="8">
         <f>Sheet1!P19</f>
-        <v>-1.165</v>
+        <v>-1.5649999999999999</v>
       </c>
       <c r="C18" s="8">
         <f>Sheet1!Q19</f>
-        <v>-2.0300000000000002</v>
+        <v>-2.4300000000000002</v>
       </c>
       <c r="D18" s="8">
         <f>Sheet1!R19</f>
-        <v>-0.46500000000000008</v>
+        <v>-0.8650000000000001</v>
       </c>
       <c r="E18" s="8">
         <f>Sheet1!T19</f>
@@ -3119,19 +3320,19 @@
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="8">
         <f>Sheet1!O20</f>
-        <v>-2.0300000000000002</v>
+        <v>-2.4300000000000002</v>
       </c>
       <c r="B19" s="8">
         <f>Sheet1!P20</f>
-        <v>-0.35499999999999998</v>
+        <v>-0.755</v>
       </c>
       <c r="C19" s="8">
         <f>Sheet1!Q20</f>
-        <v>-2.0300000000000002</v>
+        <v>-2.4300000000000002</v>
       </c>
       <c r="D19" s="8">
         <f>Sheet1!R20</f>
-        <v>0.34499999999999997</v>
+        <v>-5.5000000000000049E-2</v>
       </c>
       <c r="E19" s="8">
         <f>Sheet1!T20</f>
@@ -3149,19 +3350,19 @@
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="8">
         <f>Sheet1!O21</f>
-        <v>-2.0300000000000002</v>
+        <v>-2.4300000000000002</v>
       </c>
       <c r="B20" s="8">
         <f>Sheet1!P21</f>
-        <v>0.45500350000000006</v>
+        <v>5.5003500000000038E-2</v>
       </c>
       <c r="C20" s="8">
         <f>Sheet1!Q21</f>
-        <v>-2.0300000000000002</v>
+        <v>-2.4300000000000002</v>
       </c>
       <c r="D20" s="8">
         <f>Sheet1!R21</f>
-        <v>1.1550034999999998</v>
+        <v>0.75500349999999994</v>
       </c>
       <c r="E20" s="8">
         <f>Sheet1!T21</f>
@@ -3179,19 +3380,19 @@
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="8">
         <f>Sheet1!O22</f>
-        <v>-2.0300000000000002</v>
+        <v>-2.4300000000000002</v>
       </c>
       <c r="B21" s="8">
         <f>Sheet1!P22</f>
-        <v>1.2650105</v>
+        <v>0.86501050000000002</v>
       </c>
       <c r="C21" s="8">
         <f>Sheet1!Q22</f>
-        <v>-2.0300000000000002</v>
+        <v>-2.4300000000000002</v>
       </c>
       <c r="D21" s="8">
         <f>Sheet1!R22</f>
-        <v>1.9650105</v>
+        <v>1.5650105000000001</v>
       </c>
       <c r="E21" s="8">
         <f>Sheet1!T22</f>
@@ -3209,19 +3410,19 @@
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="8">
         <f>Sheet1!O23</f>
-        <v>-2.0024989071186394</v>
+        <v>-2.4024989071186393</v>
       </c>
       <c r="B22" s="8">
         <f>Sheet1!P23</f>
-        <v>2.0676489570205518</v>
+        <v>1.6676489570205519</v>
       </c>
       <c r="C22" s="8">
         <f>Sheet1!Q23</f>
-        <v>-1.6525080928813609</v>
+        <v>-2.0525080928813608</v>
       </c>
       <c r="D22" s="8">
         <f>Sheet1!R23</f>
-        <v>2.6738720429794478</v>
+        <v>2.2738720429794479</v>
       </c>
       <c r="E22" s="8">
         <f>Sheet1!T23</f>
@@ -3239,19 +3440,19 @@
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="8">
         <f>Sheet1!O24</f>
-        <v>-1.5975059071186393</v>
+        <v>-1.9975059071186392</v>
       </c>
       <c r="B23" s="8">
         <f>Sheet1!P24</f>
-        <v>2.769141957020552</v>
+        <v>2.3691419570205521</v>
       </c>
       <c r="C23" s="8">
         <f>Sheet1!Q24</f>
-        <v>-1.2475150928813608</v>
+        <v>-1.6475150928813607</v>
       </c>
       <c r="D23" s="8">
         <f>Sheet1!R24</f>
-        <v>3.3753650429794479</v>
+        <v>2.975365042979448</v>
       </c>
       <c r="E23" s="8">
         <f>Sheet1!T24</f>
@@ -3269,19 +3470,19 @@
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="8">
         <f>Sheet1!O25</f>
-        <v>-1.1650105000000002</v>
+        <v>-1.5650105000000001</v>
       </c>
       <c r="B24" s="8">
         <f>Sheet1!P25</f>
-        <v>3.423</v>
+        <v>3.0230000000000001</v>
       </c>
       <c r="C24" s="8">
         <f>Sheet1!Q25</f>
-        <v>-0.46501049999999999</v>
+        <v>-0.86501050000000002</v>
       </c>
       <c r="D24" s="8">
         <f>Sheet1!R25</f>
-        <v>3.423</v>
+        <v>3.0230000000000001</v>
       </c>
       <c r="E24" s="8">
         <f>Sheet1!T25</f>
@@ -3299,19 +3500,19 @@
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="8">
         <f>Sheet1!O26</f>
-        <v>-0.35500349999999992</v>
+        <v>-0.75500349999999994</v>
       </c>
       <c r="B25" s="8">
         <f>Sheet1!P26</f>
-        <v>3.423</v>
+        <v>3.0230000000000001</v>
       </c>
       <c r="C25" s="8">
         <f>Sheet1!Q26</f>
-        <v>0.34499649999999998</v>
+        <v>-5.5003500000000038E-2</v>
       </c>
       <c r="D25" s="8">
         <f>Sheet1!R26</f>
-        <v>3.423</v>
+        <v>3.0230000000000001</v>
       </c>
       <c r="E25" s="8">
         <f>Sheet1!T26</f>
@@ -3324,6 +3525,133 @@
       <c r="G25" s="8">
         <f>Sheet1!M26</f>
         <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{567D5B5A-9C87-9646-89FF-4FAA61FFF96D}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="str">
+        <f>Sheet1!A36</f>
+        <v>Point</v>
+      </c>
+      <c r="B1" t="str">
+        <f>Sheet1!B36</f>
+        <v>x1</v>
+      </c>
+      <c r="C1" t="str">
+        <f>Sheet1!C36</f>
+        <v>y1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <f>Sheet1!A37</f>
+        <v>1</v>
+      </c>
+      <c r="B2" s="8">
+        <f>Sheet1!E37</f>
+        <v>-1.6200140000000001</v>
+      </c>
+      <c r="C2" s="8">
+        <f>Sheet1!F37</f>
+        <v>3.0230000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <f>Sheet1!A38</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="8">
+        <f>Sheet1!E38</f>
+        <v>1.62</v>
+      </c>
+      <c r="C3" s="8">
+        <f>Sheet1!F38</f>
+        <v>3.0230000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <f>Sheet1!A39</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="8">
+        <f>Sheet1!E39</f>
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="C4" s="8">
+        <f>Sheet1!F39</f>
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <f>Sheet1!A40</f>
+        <v>4</v>
+      </c>
+      <c r="B5" s="8">
+        <f>Sheet1!E40</f>
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="C5" s="8">
+        <f>Sheet1!F40</f>
+        <v>-1.6200140000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <f>Sheet1!A41</f>
+        <v>5</v>
+      </c>
+      <c r="B6" s="8">
+        <f>Sheet1!E41</f>
+        <v>1.6200140000000001</v>
+      </c>
+      <c r="C6" s="8">
+        <f>Sheet1!F41</f>
+        <v>-3.0230000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <f>Sheet1!A42</f>
+        <v>6</v>
+      </c>
+      <c r="B7" s="8">
+        <f>Sheet1!E42</f>
+        <v>-1.62</v>
+      </c>
+      <c r="C7" s="8">
+        <f>Sheet1!F42</f>
+        <v>-3.0230000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <f>Sheet1!A43</f>
+        <v>7</v>
+      </c>
+      <c r="B8" s="8">
+        <f>Sheet1!E43</f>
+        <v>-2.4300000000000002</v>
+      </c>
+      <c r="C8" s="8">
+        <f>Sheet1!F43</f>
+        <v>-1.62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>